<commit_message>
updated one more test case
</commit_message>
<xml_diff>
--- a/testdata/websiteTestData.xlsx
+++ b/testdata/websiteTestData.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="search" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="fillForm" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t xml:space="preserve">searchValues</t>
   </si>
@@ -29,14 +30,45 @@
   </si>
   <si>
     <t xml:space="preserve">Toasters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form Parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nellore.mahesh867@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Breville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">900 Hamlin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sunnyvale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">94089</t>
+  </si>
+  <si>
+    <t xml:space="preserve">California</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(541) 754-3010</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -62,7 +94,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -73,6 +105,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEEEEEE"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CCFF"/>
+        <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -110,13 +148,29 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -198,14 +252,15 @@
   </sheetPr>
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.1887755102041"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -232,4 +287,84 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="26.0510204081633"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="nellore.mahesh867@gmail.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added one more sheet ini test data
</commit_message>
<xml_diff>
--- a/testdata/websiteTestData.xlsx
+++ b/testdata/websiteTestData.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="search" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="fillForm" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="checkOutAsGuest" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t xml:space="preserve">searchValues</t>
   </si>
@@ -60,6 +61,42 @@
   </si>
   <si>
     <t xml:space="preserve">(541) 754-3010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firstname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adddress1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nellore.mahesh878@gmai.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mahesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
   </si>
 </sst>
 </file>
@@ -70,7 +107,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -93,8 +130,22 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -113,8 +164,14 @@
         <bgColor rgb="FF33CCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -122,6 +179,13 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -148,7 +212,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -171,6 +235,18 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -198,7 +274,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFB2B2B2"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -258,9 +334,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.3877551020408"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -296,13 +371,14 @@
   </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="26.0510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="25.6479591836735"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,4 +443,95 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="45.015306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="2" style="2" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="16.6683673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="nellore.mahesh878@gmai.com"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>